<commit_message>
Ajuste de motor escaleta MA_11_05_CO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion05/Escaleta_MA_11_05_CO.xlsx
+++ b/fuentes/contenidos/grado11/guion05/Escaleta_MA_11_05_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Documents\Aula Planeta Colombia\Repositorios\Matematicas\fuentes\contenidos\grado11\guion05\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado11\guion05\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1125,16 +1125,34 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1174,24 +1192,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1500,128 +1500,127 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R23" sqref="R23:U23"/>
+      <selection pane="bottomLeft" activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.1328125" defaultRowHeight="14.35" customHeight="1" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.140625" defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.73046875" style="20" customWidth="1"/>
-    <col min="2" max="2" width="13.53125" style="20" customWidth="1"/>
-    <col min="3" max="3" width="13.59765625" style="20" customWidth="1"/>
-    <col min="4" max="4" width="21.73046875" style="20" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" style="20" customWidth="1"/>
-    <col min="6" max="6" width="11.73046875" style="21" customWidth="1"/>
-    <col min="7" max="7" width="15.73046875" style="20" customWidth="1"/>
-    <col min="8" max="8" width="8.265625" style="21" customWidth="1"/>
-    <col min="9" max="9" width="6.73046875" style="21" customWidth="1"/>
-    <col min="10" max="10" width="15.73046875" style="20" customWidth="1"/>
-    <col min="11" max="11" width="12.59765625" style="20" customWidth="1"/>
-    <col min="12" max="12" width="9.59765625" style="20" customWidth="1"/>
-    <col min="13" max="13" width="7.73046875" style="20" customWidth="1"/>
-    <col min="14" max="14" width="7.86328125" style="20" customWidth="1"/>
-    <col min="15" max="15" width="51.73046875" style="21" customWidth="1"/>
-    <col min="16" max="16" width="5.19921875" style="21" customWidth="1"/>
-    <col min="17" max="17" width="2.265625" style="21" customWidth="1"/>
-    <col min="18" max="18" width="4.3984375" style="20" customWidth="1"/>
-    <col min="19" max="19" width="10.59765625" style="20" customWidth="1"/>
-    <col min="20" max="20" width="17.53125" style="20" customWidth="1"/>
-    <col min="21" max="21" width="13.59765625" style="20" customWidth="1"/>
-    <col min="22" max="16384" width="14.1328125" style="20"/>
+    <col min="1" max="1" width="9.7109375" style="20" customWidth="1"/>
+    <col min="2" max="3" width="13.5703125" style="20" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" style="20" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" style="20" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="21" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="20" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" style="21" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" style="21" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" style="20" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" style="20" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" style="20" customWidth="1"/>
+    <col min="13" max="13" width="7.7109375" style="20" customWidth="1"/>
+    <col min="14" max="14" width="7.85546875" style="20" customWidth="1"/>
+    <col min="15" max="15" width="51.7109375" style="21" customWidth="1"/>
+    <col min="16" max="16" width="5.140625" style="21" customWidth="1"/>
+    <col min="17" max="17" width="2.28515625" style="21" customWidth="1"/>
+    <col min="18" max="18" width="4.42578125" style="20" customWidth="1"/>
+    <col min="19" max="19" width="10.5703125" style="20" customWidth="1"/>
+    <col min="20" max="20" width="17.5703125" style="20" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" style="20" customWidth="1"/>
+    <col min="22" max="16384" width="14.140625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="3" customFormat="1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:21" s="3" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="47" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="F1" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="43" t="s">
+      <c r="G1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="35" t="s">
+      <c r="H1" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="I1" s="43" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="47" t="s">
+      <c r="J1" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="45" t="s">
+      <c r="K1" s="51" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="43" t="s">
+      <c r="L1" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="49" t="s">
+      <c r="M1" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="49"/>
-      <c r="O1" s="37" t="s">
+      <c r="N1" s="55"/>
+      <c r="O1" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="37" t="s">
+      <c r="P1" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="52" t="s">
+      <c r="Q1" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="56" t="s">
+      <c r="R1" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="52" t="s">
+      <c r="S1" s="37" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="54" t="s">
+      <c r="T1" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="52" t="s">
+      <c r="U1" s="37" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="3" customFormat="1" ht="14.35" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="42"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="44"/>
+    <row r="2" spans="1:21" s="3" customFormat="1" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="48"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="50"/>
       <c r="M2" s="22" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="53"/>
-      <c r="R2" s="57"/>
-      <c r="S2" s="53"/>
-      <c r="T2" s="55"/>
-      <c r="U2" s="53"/>
-    </row>
-    <row r="3" spans="1:21" s="4" customFormat="1" ht="14.35" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="42"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="38"/>
+    </row>
+    <row r="3" spans="1:21" s="4" customFormat="1" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
         <v>15</v>
       </c>
@@ -1680,7 +1679,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="4" customFormat="1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
         <v>15</v>
       </c>
@@ -1741,7 +1740,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:21" s="4" customFormat="1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
         <v>15</v>
       </c>
@@ -1802,7 +1801,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="4" customFormat="1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:21" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
         <v>15</v>
       </c>
@@ -1863,7 +1862,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:21" s="4" customFormat="1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:21" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
         <v>15</v>
       </c>
@@ -1924,7 +1923,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="8" spans="1:21" s="4" customFormat="1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:21" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
         <v>15</v>
       </c>
@@ -1985,7 +1984,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="4" customFormat="1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:21" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
         <v>15</v>
       </c>
@@ -2046,7 +2045,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="4" customFormat="1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:21" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
         <v>15</v>
       </c>
@@ -2107,7 +2106,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="4" customFormat="1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:21" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
         <v>15</v>
       </c>
@@ -2168,7 +2167,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="12" spans="1:21" s="4" customFormat="1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:21" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
         <v>15</v>
       </c>
@@ -2229,7 +2228,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="13" spans="1:21" s="4" customFormat="1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:21" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
         <v>15</v>
       </c>
@@ -2290,7 +2289,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="14" spans="1:21" s="4" customFormat="1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:21" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
         <v>15</v>
       </c>
@@ -2351,7 +2350,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="15" spans="1:21" s="4" customFormat="1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:21" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
         <v>15</v>
       </c>
@@ -2412,7 +2411,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="16" spans="1:21" s="4" customFormat="1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:21" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
         <v>15</v>
       </c>
@@ -2473,7 +2472,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="17" spans="1:21" s="4" customFormat="1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:21" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
         <v>15</v>
       </c>
@@ -2534,7 +2533,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="18" spans="1:21" s="4" customFormat="1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:21" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
         <v>15</v>
       </c>
@@ -2595,7 +2594,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="1:21" s="4" customFormat="1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:21" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="23" t="s">
         <v>15</v>
       </c>
@@ -2656,7 +2655,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="1:21" s="4" customFormat="1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:21" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
         <v>15</v>
       </c>
@@ -2715,7 +2714,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="21" spans="1:21" s="4" customFormat="1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:21" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
         <v>15</v>
       </c>
@@ -2750,7 +2749,7 @@
       </c>
       <c r="M21" s="30"/>
       <c r="N21" s="30" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="O21" s="7" t="s">
         <v>215</v>
@@ -2774,7 +2773,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="22" spans="1:21" s="4" customFormat="1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:21" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="23" t="s">
         <v>15</v>
       </c>
@@ -2835,7 +2834,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:21" s="4" customFormat="1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:21" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="23" t="s">
         <v>15</v>
       </c>
@@ -2894,7 +2893,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="24" spans="1:21" s="4" customFormat="1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:21" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
         <v>15</v>
       </c>
@@ -2953,7 +2952,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="25" spans="1:21" s="4" customFormat="1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:21" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="23" t="s">
         <v>15</v>
       </c>
@@ -2998,7 +2997,7 @@
       <c r="T25" s="17"/>
       <c r="U25" s="15"/>
     </row>
-    <row r="26" spans="1:21" s="4" customFormat="1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:21" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="23" t="s">
         <v>15</v>
       </c>
@@ -3059,7 +3058,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="27" spans="1:21" s="4" customFormat="1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:21" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
         <v>15</v>
       </c>
@@ -3120,187 +3119,187 @@
         <v>143</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="42" spans="1:1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="20" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="43" spans="1:1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="20" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="44" spans="1:1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="20" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="45" spans="1:1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="20" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="46" spans="1:1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="20" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="47" spans="1:1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="20" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="48" spans="1:1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="20" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="49" spans="1:1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="20" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="50" spans="1:1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="52" spans="1:1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="53" spans="1:1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="20" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="54" spans="1:1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="20" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="55" spans="1:1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="20" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="56" spans="1:1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="20" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="57" spans="1:1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="20" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="58" spans="1:1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="20" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="59" spans="1:1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="60" spans="1:1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="20" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="61" spans="1:1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="20" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="62" spans="1:1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="20" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="63" spans="1:1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="20" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="64" spans="1:1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="20" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="20" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="66" spans="1:1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="20" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="67" spans="1:1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="20" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="68" spans="1:1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="20" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="69" spans="1:1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="20" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="70" spans="1:1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="20" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="71" spans="1:1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="20" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="72" spans="1:1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="20" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="73" spans="1:1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="20" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="74" spans="1:1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="20" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="75" spans="1:1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="20" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="76" spans="1:1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="20" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="77" spans="1:1" ht="14.35" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="20" t="s">
         <v>115</v>
       </c>
@@ -3310,12 +3309,6 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -3330,6 +3323,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3380,27 +3379,27 @@
       <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.86328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="34" style="1" customWidth="1"/>
-    <col min="5" max="5" width="34.86328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.59765625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="34.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="18" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.73046875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.59765625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" style="1" customWidth="1"/>
     <col min="12" max="12" width="17" style="1" customWidth="1"/>
-    <col min="13" max="13" width="11.3984375" style="1"/>
-    <col min="14" max="14" width="24.265625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="69.86328125" style="1" hidden="1" customWidth="1"/>
-    <col min="16" max="16384" width="11.3984375" style="1"/>
+    <col min="13" max="13" width="11.42578125" style="1"/>
+    <col min="14" max="14" width="24.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="69.85546875" style="1" hidden="1" customWidth="1"/>
+    <col min="16" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -3417,7 +3416,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -3441,7 +3440,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -3460,7 +3459,7 @@
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
     </row>
-    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -3479,7 +3478,7 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
@@ -3495,7 +3494,7 @@
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
@@ -3512,7 +3511,7 @@
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
@@ -3529,7 +3528,7 @@
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -3544,7 +3543,7 @@
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
     </row>
-    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -3559,7 +3558,7 @@
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
     </row>
-    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -3574,7 +3573,7 @@
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -3589,7 +3588,7 @@
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
     </row>
-    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -3604,7 +3603,7 @@
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -3619,7 +3618,7 @@
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
     </row>
-    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -3634,7 +3633,7 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
     </row>
-    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -3649,7 +3648,7 @@
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
     </row>
-    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -3664,7 +3663,7 @@
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
     </row>
-    <row r="17" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="1" t="s">
@@ -3678,7 +3677,7 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="1" t="s">
@@ -3692,7 +3691,7 @@
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
     </row>
-    <row r="19" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="1" t="s">
@@ -3706,7 +3705,7 @@
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
     </row>
-    <row r="20" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="1" t="s">
@@ -3720,7 +3719,7 @@
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
     </row>
-    <row r="21" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -3735,7 +3734,7 @@
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
     </row>
-    <row r="22" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -3750,7 +3749,7 @@
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
     </row>
-    <row r="23" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -3765,7 +3764,7 @@
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
     </row>
-    <row r="24" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -3780,7 +3779,7 @@
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
     </row>
-    <row r="25" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -3795,7 +3794,7 @@
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
     </row>
-    <row r="26" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -3810,7 +3809,7 @@
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="27" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -3825,7 +3824,7 @@
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
     </row>
-    <row r="28" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -3840,7 +3839,7 @@
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="29" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -3855,7 +3854,7 @@
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -3870,7 +3869,7 @@
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -3885,7 +3884,7 @@
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
     </row>
-    <row r="32" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -3900,7 +3899,7 @@
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
     </row>
-    <row r="33" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -3915,7 +3914,7 @@
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
     </row>
-    <row r="34" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="34" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -3930,7 +3929,7 @@
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
     </row>
-    <row r="35" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="35" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -3945,7 +3944,7 @@
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
     </row>
-    <row r="36" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="36" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -3960,7 +3959,7 @@
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
     </row>
-    <row r="37" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="37" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -3975,7 +3974,7 @@
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
     </row>
-    <row r="38" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="38" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -3990,7 +3989,7 @@
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
     </row>
-    <row r="39" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="39" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -4005,7 +4004,7 @@
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
     </row>
-    <row r="40" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="40" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
@@ -4020,7 +4019,7 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
     </row>
-    <row r="41" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="41" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
@@ -4035,7 +4034,7 @@
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
     </row>
-    <row r="42" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="42" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
@@ -4050,7 +4049,7 @@
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
     </row>
-    <row r="43" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="43" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
@@ -4065,7 +4064,7 @@
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
     </row>
-    <row r="44" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="44" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
@@ -4080,7 +4079,7 @@
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
     </row>
-    <row r="45" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="45" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
@@ -4095,7 +4094,7 @@
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
     </row>
-    <row r="46" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="46" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -4110,7 +4109,7 @@
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
     </row>
-    <row r="47" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="47" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
@@ -4125,7 +4124,7 @@
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
     </row>
-    <row r="48" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="48" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
@@ -4140,7 +4139,7 @@
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
     </row>
-    <row r="49" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="49" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
@@ -4152,7 +4151,7 @@
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
     </row>
-    <row r="50" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="50" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -4164,7 +4163,7 @@
       <c r="K50" s="2"/>
       <c r="L50" s="2"/>
     </row>
-    <row r="51" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="51" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
@@ -4177,7 +4176,7 @@
       <c r="K51" s="2"/>
       <c r="L51" s="2"/>
     </row>
-    <row r="52" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="52" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
@@ -4190,7 +4189,7 @@
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
     </row>
-    <row r="53" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="53" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
@@ -4203,7 +4202,7 @@
       <c r="K53" s="2"/>
       <c r="L53" s="2"/>
     </row>
-    <row r="54" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="54" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
@@ -4216,7 +4215,7 @@
       <c r="K54" s="2"/>
       <c r="L54" s="2"/>
     </row>
-    <row r="55" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="55" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
@@ -4229,7 +4228,7 @@
       <c r="K55" s="2"/>
       <c r="L55" s="2"/>
     </row>
-    <row r="56" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="56" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
@@ -4242,7 +4241,7 @@
       <c r="K56" s="2"/>
       <c r="L56" s="2"/>
     </row>
-    <row r="57" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="57" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
@@ -4255,7 +4254,7 @@
       <c r="K57" s="2"/>
       <c r="L57" s="2"/>
     </row>
-    <row r="58" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="58" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
@@ -4268,7 +4267,7 @@
       <c r="K58" s="2"/>
       <c r="L58" s="2"/>
     </row>
-    <row r="59" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="59" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
@@ -4281,7 +4280,7 @@
       <c r="K59" s="2"/>
       <c r="L59" s="2"/>
     </row>
-    <row r="60" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="60" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
@@ -4294,7 +4293,7 @@
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
     </row>
-    <row r="61" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="61" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
@@ -4307,7 +4306,7 @@
       <c r="K61" s="2"/>
       <c r="L61" s="2"/>
     </row>
-    <row r="62" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="62" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
@@ -4320,7 +4319,7 @@
       <c r="K62" s="2"/>
       <c r="L62" s="2"/>
     </row>
-    <row r="63" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="63" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
@@ -4333,7 +4332,7 @@
       <c r="K63" s="2"/>
       <c r="L63" s="2"/>
     </row>
-    <row r="64" spans="2:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="64" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
@@ -4346,7 +4345,7 @@
       <c r="K64" s="2"/>
       <c r="L64" s="2"/>
     </row>
-    <row r="65" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="65" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
@@ -4359,7 +4358,7 @@
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
     </row>
-    <row r="66" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="66" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
@@ -4372,7 +4371,7 @@
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
     </row>
-    <row r="67" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="67" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
@@ -4385,7 +4384,7 @@
       <c r="K67" s="2"/>
       <c r="L67" s="2"/>
     </row>
-    <row r="68" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="68" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
@@ -4398,7 +4397,7 @@
       <c r="K68" s="2"/>
       <c r="L68" s="2"/>
     </row>
-    <row r="69" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="69" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
@@ -4411,7 +4410,7 @@
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
     </row>
-    <row r="70" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="70" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
@@ -4424,7 +4423,7 @@
       <c r="K70" s="2"/>
       <c r="L70" s="2"/>
     </row>
-    <row r="71" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="71" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -4438,7 +4437,7 @@
       <c r="K71" s="2"/>
       <c r="L71" s="2"/>
     </row>
-    <row r="72" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="72" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -4452,7 +4451,7 @@
       <c r="K72" s="2"/>
       <c r="L72" s="2"/>
     </row>
-    <row r="73" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -4466,7 +4465,7 @@
       <c r="K73" s="2"/>
       <c r="L73" s="2"/>
     </row>
-    <row r="74" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="74" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -4480,7 +4479,7 @@
       <c r="K74" s="2"/>
       <c r="L74" s="2"/>
     </row>
-    <row r="75" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="75" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -4494,7 +4493,7 @@
       <c r="K75" s="2"/>
       <c r="L75" s="2"/>
     </row>
-    <row r="76" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="76" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -4508,7 +4507,7 @@
       <c r="K76" s="2"/>
       <c r="L76" s="2"/>
     </row>
-    <row r="77" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="77" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -4522,7 +4521,7 @@
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
     </row>
-    <row r="78" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="78" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -4536,7 +4535,7 @@
       <c r="K78" s="2"/>
       <c r="L78" s="2"/>
     </row>
-    <row r="79" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="79" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -4550,7 +4549,7 @@
       <c r="K79" s="2"/>
       <c r="L79" s="2"/>
     </row>
-    <row r="80" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="80" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -4564,7 +4563,7 @@
       <c r="K80" s="2"/>
       <c r="L80" s="2"/>
     </row>
-    <row r="81" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="81" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -4578,7 +4577,7 @@
       <c r="K81" s="2"/>
       <c r="L81" s="2"/>
     </row>
-    <row r="82" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="82" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -4592,7 +4591,7 @@
       <c r="K82" s="2"/>
       <c r="L82" s="2"/>
     </row>
-    <row r="83" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="83" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -4606,7 +4605,7 @@
       <c r="K83" s="2"/>
       <c r="L83" s="2"/>
     </row>
-    <row r="84" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="84" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -4620,7 +4619,7 @@
       <c r="K84" s="2"/>
       <c r="L84" s="2"/>
     </row>
-    <row r="85" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="85" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -4634,7 +4633,7 @@
       <c r="K85" s="2"/>
       <c r="L85" s="2"/>
     </row>
-    <row r="86" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="86" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -4648,7 +4647,7 @@
       <c r="K86" s="2"/>
       <c r="L86" s="2"/>
     </row>
-    <row r="87" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="87" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -4662,7 +4661,7 @@
       <c r="K87" s="2"/>
       <c r="L87" s="2"/>
     </row>
-    <row r="88" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="88" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -4676,7 +4675,7 @@
       <c r="K88" s="2"/>
       <c r="L88" s="2"/>
     </row>
-    <row r="89" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="89" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -4690,7 +4689,7 @@
       <c r="K89" s="2"/>
       <c r="L89" s="2"/>
     </row>
-    <row r="90" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="90" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -4704,7 +4703,7 @@
       <c r="K90" s="2"/>
       <c r="L90" s="2"/>
     </row>
-    <row r="91" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="91" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
@@ -4718,7 +4717,7 @@
       <c r="K91" s="2"/>
       <c r="L91" s="2"/>
     </row>
-    <row r="92" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="92" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
@@ -4732,7 +4731,7 @@
       <c r="K92" s="2"/>
       <c r="L92" s="2"/>
     </row>
-    <row r="93" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="93" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
@@ -4746,7 +4745,7 @@
       <c r="K93" s="2"/>
       <c r="L93" s="2"/>
     </row>
-    <row r="94" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="94" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
@@ -4760,7 +4759,7 @@
       <c r="K94" s="2"/>
       <c r="L94" s="2"/>
     </row>
-    <row r="95" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="95" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
@@ -4774,7 +4773,7 @@
       <c r="K95" s="2"/>
       <c r="L95" s="2"/>
     </row>
-    <row r="96" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="96" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="2"/>
       <c r="C96" s="2"/>
@@ -4788,7 +4787,7 @@
       <c r="K96" s="2"/>
       <c r="L96" s="2"/>
     </row>
-    <row r="97" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="97" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="2"/>
       <c r="C97" s="2"/>
@@ -4802,7 +4801,7 @@
       <c r="K97" s="2"/>
       <c r="L97" s="2"/>
     </row>
-    <row r="98" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="98" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
@@ -4816,7 +4815,7 @@
       <c r="K98" s="2"/>
       <c r="L98" s="2"/>
     </row>
-    <row r="99" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="99" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2"/>
@@ -4830,7 +4829,7 @@
       <c r="K99" s="2"/>
       <c r="L99" s="2"/>
     </row>
-    <row r="100" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="100" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2"/>
@@ -4844,7 +4843,7 @@
       <c r="K100" s="2"/>
       <c r="L100" s="2"/>
     </row>
-    <row r="101" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="101" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="2"/>
       <c r="C101" s="2"/>
@@ -4858,7 +4857,7 @@
       <c r="K101" s="2"/>
       <c r="L101" s="2"/>
     </row>
-    <row r="102" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="102" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
       <c r="B102" s="2"/>
       <c r="C102" s="2"/>
@@ -4872,7 +4871,7 @@
       <c r="K102" s="2"/>
       <c r="L102" s="2"/>
     </row>
-    <row r="103" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="103" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
       <c r="B103" s="2"/>
       <c r="C103" s="2"/>
@@ -4886,7 +4885,7 @@
       <c r="K103" s="2"/>
       <c r="L103" s="2"/>
     </row>
-    <row r="104" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="104" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
       <c r="B104" s="2"/>
       <c r="C104" s="2"/>
@@ -4900,7 +4899,7 @@
       <c r="K104" s="2"/>
       <c r="L104" s="2"/>
     </row>
-    <row r="105" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="105" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
       <c r="B105" s="2"/>
       <c r="C105" s="2"/>
@@ -4914,7 +4913,7 @@
       <c r="K105" s="2"/>
       <c r="L105" s="2"/>
     </row>
-    <row r="106" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="106" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -4928,7 +4927,7 @@
       <c r="K106" s="2"/>
       <c r="L106" s="2"/>
     </row>
-    <row r="107" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="107" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
       <c r="B107" s="2"/>
       <c r="C107" s="2"/>
@@ -4942,7 +4941,7 @@
       <c r="K107" s="2"/>
       <c r="L107" s="2"/>
     </row>
-    <row r="108" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="108" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
@@ -4956,7 +4955,7 @@
       <c r="K108" s="2"/>
       <c r="L108" s="2"/>
     </row>
-    <row r="109" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="109" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
@@ -4970,7 +4969,7 @@
       <c r="K109" s="2"/>
       <c r="L109" s="2"/>
     </row>
-    <row r="110" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="110" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
       <c r="B110" s="2"/>
       <c r="C110" s="2"/>
@@ -4984,7 +4983,7 @@
       <c r="K110" s="2"/>
       <c r="L110" s="2"/>
     </row>
-    <row r="111" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="111" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
       <c r="B111" s="2"/>
       <c r="C111" s="2"/>
@@ -4998,7 +4997,7 @@
       <c r="K111" s="2"/>
       <c r="L111" s="2"/>
     </row>
-    <row r="112" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="112" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
       <c r="B112" s="2"/>
       <c r="C112" s="2"/>
@@ -5012,7 +5011,7 @@
       <c r="K112" s="2"/>
       <c r="L112" s="2"/>
     </row>
-    <row r="113" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="113" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
       <c r="B113" s="2"/>
       <c r="C113" s="2"/>
@@ -5026,7 +5025,7 @@
       <c r="K113" s="2"/>
       <c r="L113" s="2"/>
     </row>
-    <row r="114" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="114" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
       <c r="B114" s="2"/>
       <c r="C114" s="2"/>
@@ -5040,7 +5039,7 @@
       <c r="K114" s="2"/>
       <c r="L114" s="2"/>
     </row>
-    <row r="115" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="115" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="2"/>
       <c r="B115" s="2"/>
       <c r="C115" s="2"/>
@@ -5054,7 +5053,7 @@
       <c r="K115" s="2"/>
       <c r="L115" s="2"/>
     </row>
-    <row r="116" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="116" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="2"/>
       <c r="B116" s="2"/>
       <c r="C116" s="2"/>
@@ -5068,7 +5067,7 @@
       <c r="K116" s="2"/>
       <c r="L116" s="2"/>
     </row>
-    <row r="117" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="117" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="2"/>
       <c r="B117" s="2"/>
       <c r="C117" s="2"/>
@@ -5082,7 +5081,7 @@
       <c r="K117" s="2"/>
       <c r="L117" s="2"/>
     </row>
-    <row r="118" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="118" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="2"/>
       <c r="B118" s="2"/>
       <c r="C118" s="2"/>
@@ -5096,7 +5095,7 @@
       <c r="K118" s="2"/>
       <c r="L118" s="2"/>
     </row>
-    <row r="119" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="119" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -5110,7 +5109,7 @@
       <c r="K119" s="2"/>
       <c r="L119" s="2"/>
     </row>
-    <row r="120" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="120" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="2"/>
       <c r="B120" s="2"/>
       <c r="C120" s="2"/>
@@ -5124,7 +5123,7 @@
       <c r="K120" s="2"/>
       <c r="L120" s="2"/>
     </row>
-    <row r="121" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="121" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="2"/>
       <c r="B121" s="2"/>
       <c r="C121" s="2"/>
@@ -5138,7 +5137,7 @@
       <c r="K121" s="2"/>
       <c r="L121" s="2"/>
     </row>
-    <row r="122" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="122" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A122" s="2"/>
       <c r="B122" s="2"/>
       <c r="C122" s="2"/>
@@ -5152,7 +5151,7 @@
       <c r="K122" s="2"/>
       <c r="L122" s="2"/>
     </row>
-    <row r="123" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="123" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="2"/>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -5166,7 +5165,7 @@
       <c r="K123" s="2"/>
       <c r="L123" s="2"/>
     </row>
-    <row r="124" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="124" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="2"/>
       <c r="B124" s="2"/>
       <c r="C124" s="2"/>
@@ -5180,7 +5179,7 @@
       <c r="K124" s="2"/>
       <c r="L124" s="2"/>
     </row>
-    <row r="125" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="125" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
       <c r="C125" s="2"/>
@@ -5194,7 +5193,7 @@
       <c r="K125" s="2"/>
       <c r="L125" s="2"/>
     </row>
-    <row r="126" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="126" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="2"/>
       <c r="B126" s="2"/>
       <c r="C126" s="2"/>
@@ -5208,7 +5207,7 @@
       <c r="K126" s="2"/>
       <c r="L126" s="2"/>
     </row>
-    <row r="127" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="127" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A127" s="2"/>
       <c r="B127" s="2"/>
       <c r="C127" s="2"/>
@@ -5222,7 +5221,7 @@
       <c r="K127" s="2"/>
       <c r="L127" s="2"/>
     </row>
-    <row r="128" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="128" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="2"/>
       <c r="B128" s="2"/>
       <c r="C128" s="2"/>
@@ -5236,7 +5235,7 @@
       <c r="K128" s="2"/>
       <c r="L128" s="2"/>
     </row>
-    <row r="129" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="129" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="2"/>
       <c r="B129" s="2"/>
       <c r="C129" s="2"/>
@@ -5250,7 +5249,7 @@
       <c r="K129" s="2"/>
       <c r="L129" s="2"/>
     </row>
-    <row r="130" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="130" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130" s="2"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2"/>
@@ -5264,7 +5263,7 @@
       <c r="K130" s="2"/>
       <c r="L130" s="2"/>
     </row>
-    <row r="131" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="131" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A131" s="2"/>
       <c r="B131" s="2"/>
       <c r="C131" s="2"/>
@@ -5278,7 +5277,7 @@
       <c r="K131" s="2"/>
       <c r="L131" s="2"/>
     </row>
-    <row r="132" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="132" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A132" s="2"/>
       <c r="B132" s="2"/>
       <c r="C132" s="2"/>
@@ -5292,7 +5291,7 @@
       <c r="K132" s="2"/>
       <c r="L132" s="2"/>
     </row>
-    <row r="133" spans="1:12" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="133" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A133" s="2"/>
       <c r="B133" s="2"/>
       <c r="C133" s="2"/>

</xml_diff>

<commit_message>
Ajuste de escaleta MA_11_05_CO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion05/Escaleta_MA_11_05_CO.xlsx
+++ b/fuentes/contenidos/grado11/guion05/Escaleta_MA_11_05_CO.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="249">
   <si>
     <t>Asignatura</t>
   </si>
@@ -1029,7 +1029,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1119,40 +1119,19 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1192,6 +1171,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1500,125 +1497,111 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H25" sqref="H25"/>
+      <selection pane="bottomLeft" activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.140625" defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="50.140625" defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="20" customWidth="1"/>
-    <col min="2" max="3" width="13.5703125" style="20" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" style="20" customWidth="1"/>
-    <col min="5" max="5" width="22.28515625" style="20" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="21" customWidth="1"/>
-    <col min="7" max="7" width="41.85546875" style="20" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" style="21" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="21" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" style="20" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" style="20" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" style="20" customWidth="1"/>
-    <col min="13" max="13" width="7.7109375" style="20" customWidth="1"/>
-    <col min="14" max="14" width="7.85546875" style="20" customWidth="1"/>
-    <col min="15" max="15" width="51.7109375" style="21" customWidth="1"/>
-    <col min="16" max="16" width="11.28515625" style="21" customWidth="1"/>
-    <col min="17" max="17" width="2.28515625" style="21" customWidth="1"/>
-    <col min="18" max="18" width="4.42578125" style="20" customWidth="1"/>
-    <col min="19" max="19" width="10.5703125" style="20" customWidth="1"/>
-    <col min="20" max="20" width="17.5703125" style="20" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" style="20" customWidth="1"/>
-    <col min="22" max="16384" width="14.140625" style="20"/>
+    <col min="1" max="5" width="50.140625" style="20"/>
+    <col min="6" max="6" width="50.140625" style="21"/>
+    <col min="7" max="7" width="50.140625" style="20"/>
+    <col min="8" max="9" width="50.140625" style="21"/>
+    <col min="10" max="14" width="50.140625" style="20"/>
+    <col min="15" max="17" width="50.140625" style="21"/>
+    <col min="18" max="16384" width="50.140625" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="3" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="56" t="s">
+      <c r="C1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="38" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="43" t="s">
+      <c r="F1" s="34" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="49" t="s">
+      <c r="G1" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="43" t="s">
+      <c r="H1" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="43" t="s">
+      <c r="I1" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="53" t="s">
+      <c r="J1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="51" t="s">
+      <c r="K1" s="44" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="49" t="s">
+      <c r="L1" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="55" t="s">
+      <c r="M1" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="55"/>
-      <c r="O1" s="35" t="s">
+      <c r="N1" s="48"/>
+      <c r="O1" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="35" t="s">
+      <c r="P1" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="37" t="s">
+      <c r="Q1" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="41" t="s">
+      <c r="R1" s="55" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="37" t="s">
+      <c r="S1" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="39" t="s">
+      <c r="T1" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="37" t="s">
+      <c r="U1" s="51" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="3" customFormat="1" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="48"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="50"/>
+      <c r="A2" s="41"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="43"/>
       <c r="M2" s="22" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="42"/>
-      <c r="S2" s="38"/>
-      <c r="T2" s="40"/>
-      <c r="U2" s="38"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="52"/>
+      <c r="R2" s="56"/>
+      <c r="S2" s="52"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="52"/>
     </row>
     <row r="3" spans="1:21" s="4" customFormat="1" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
@@ -1642,7 +1625,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J3" s="9" t="s">
         <v>167</v>
@@ -1703,7 +1686,7 @@
         <v>2</v>
       </c>
       <c r="I4" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>156</v>
@@ -1764,7 +1747,7 @@
         <v>3</v>
       </c>
       <c r="I5" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>160</v>
@@ -1825,7 +1808,7 @@
         <v>4</v>
       </c>
       <c r="I6" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J6" s="9" t="s">
         <v>162</v>
@@ -1947,7 +1930,7 @@
         <v>6</v>
       </c>
       <c r="I8" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J8" s="9" t="s">
         <v>165</v>
@@ -2008,7 +1991,7 @@
         <v>7</v>
       </c>
       <c r="I9" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J9" s="9" t="s">
         <v>172</v>
@@ -2069,7 +2052,7 @@
         <v>8</v>
       </c>
       <c r="I10" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J10" s="9" t="s">
         <v>171</v>
@@ -2130,7 +2113,7 @@
         <v>9</v>
       </c>
       <c r="I11" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J11" s="9" t="s">
         <v>177</v>
@@ -2191,7 +2174,7 @@
         <v>10</v>
       </c>
       <c r="I12" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J12" s="9" t="s">
         <v>180</v>
@@ -2252,7 +2235,7 @@
         <v>11</v>
       </c>
       <c r="I13" s="27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J13" s="9" t="s">
         <v>245</v>
@@ -2313,7 +2296,7 @@
         <v>12</v>
       </c>
       <c r="I14" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J14" s="9" t="s">
         <v>246</v>
@@ -2374,7 +2357,7 @@
         <v>13</v>
       </c>
       <c r="I15" s="27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J15" s="9" t="s">
         <v>152</v>
@@ -2435,7 +2418,7 @@
         <v>14</v>
       </c>
       <c r="I16" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J16" s="9" t="s">
         <v>199</v>
@@ -2557,7 +2540,7 @@
         <v>16</v>
       </c>
       <c r="I18" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J18" s="9" t="s">
         <v>205</v>
@@ -2618,7 +2601,7 @@
         <v>17</v>
       </c>
       <c r="I19" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J19" s="9" t="s">
         <v>208</v>
@@ -2797,7 +2780,7 @@
         <v>20</v>
       </c>
       <c r="I22" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J22" s="9" t="s">
         <v>217</v>
@@ -2858,7 +2841,7 @@
         <v>21</v>
       </c>
       <c r="I23" s="27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J23" s="9" t="s">
         <v>193</v>
@@ -2914,8 +2897,8 @@
       <c r="H24" s="26">
         <v>22</v>
       </c>
-      <c r="I24" s="31" t="s">
-        <v>20</v>
+      <c r="I24" s="27" t="s">
+        <v>19</v>
       </c>
       <c r="J24" s="13" t="s">
         <v>195</v>
@@ -2975,7 +2958,9 @@
       <c r="H25" s="26">
         <v>23</v>
       </c>
-      <c r="I25" s="33"/>
+      <c r="I25" s="27" t="s">
+        <v>19</v>
+      </c>
       <c r="J25" s="18" t="s">
         <v>190</v>
       </c>
@@ -2985,8 +2970,8 @@
       <c r="L25" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="M25" s="34"/>
-      <c r="N25" s="34"/>
+      <c r="M25" s="33"/>
+      <c r="N25" s="33"/>
       <c r="O25" s="19"/>
       <c r="P25" s="14" t="s">
         <v>19</v>
@@ -3020,8 +3005,8 @@
       <c r="H26" s="26">
         <v>24</v>
       </c>
-      <c r="I26" s="33" t="s">
-        <v>20</v>
+      <c r="I26" s="27" t="s">
+        <v>19</v>
       </c>
       <c r="J26" s="18" t="s">
         <v>188</v>
@@ -3032,8 +3017,8 @@
       <c r="L26" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="M26" s="34"/>
-      <c r="N26" s="34" t="s">
+      <c r="M26" s="33"/>
+      <c r="N26" s="33" t="s">
         <v>103</v>
       </c>
       <c r="O26" s="19" t="s">
@@ -3081,7 +3066,7 @@
       <c r="H27" s="26">
         <v>25</v>
       </c>
-      <c r="I27" s="33" t="s">
+      <c r="I27" s="27" t="s">
         <v>20</v>
       </c>
       <c r="J27" s="18" t="s">
@@ -3093,8 +3078,8 @@
       <c r="L27" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="M27" s="34"/>
-      <c r="N27" s="34" t="s">
+      <c r="M27" s="33"/>
+      <c r="N27" s="33" t="s">
         <v>83</v>
       </c>
       <c r="O27" s="19" t="s">
@@ -3309,6 +3294,12 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -3323,12 +3314,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3351,7 +3336,7 @@
           <x14:formula1>
             <xm:f>DATOS!$D$1:$D$2</xm:f>
           </x14:formula1>
-          <xm:sqref>I3:I27 P3:P27 K3:K27</xm:sqref>
+          <xm:sqref>K3:K27 P3:P27 I3:I27</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>

<commit_message>
Ajuste de escaleta mat11_05
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado11/guion05/Escaleta_MA_11_05_CO.xlsx
+++ b/fuentes/contenidos/grado11/guion05/Escaleta_MA_11_05_CO.xlsx
@@ -567,9 +567,6 @@
     <t>Refuerza tu aprendizaje: El área bajo la curva</t>
   </si>
   <si>
-    <t>Actividad en la que se revisa la claridad en la aplicabilidad de los métodos</t>
-  </si>
-  <si>
     <t xml:space="preserve">Plantear al menos ocho y máximo diez ejercicios, en los que el estudiante pueda evidenciar una correcta toma de decisiones para aplicar uno u otro método de integración. Preguntar por ejemplo las características que ha de tener una función para que pueda aplicarse el método de sustitución, que expresen en sus palabras qué significan u, v, du y dv en la integración por partes, dada una función cuál método aplicaría para integrarla, etc. </t>
   </si>
   <si>
@@ -610,9 +607,6 @@
   </si>
   <si>
     <t>Competencias: El área entre dos funciones</t>
-  </si>
-  <si>
-    <t>Actividad para generalizar el área entre curvas</t>
   </si>
   <si>
     <t>Partir de un problema real aosciado por ejemplo con el cuidado de la salud o el bienestar o con otros campos en el que se requiera clacular el área entre dos funciones. En el motor F13 deben incluirse pestañas para introducir el problema, de qué manera ello trastocó la notación de los límites de la integral, el cálculo usando software concreto (por ejemplo Geogebra, Mathematica, Derive,  etc.) Explicitar los mecanismos de solución, solucionar completamente el problema y proponer uno a los estudiantes.</t>
@@ -716,9 +710,6 @@
     <t>Plantear 10 preguntas abiertas respecto a problemas cotidianos o situaciones problema como las planteadas en los recursos previos en las que se haga evidente la conexión entre derivadas e integrales. Por ejemplo en relaciones entre la razón de cambio instantanea en velocidad y su conexión con aceleración y desplazamiento, las relaciones entre fórmulas conocidas de cálculo de magnitudes como la de que la integral de la longitud es el área y la integral del área el volumen, etc.</t>
   </si>
   <si>
-    <t>Significado de sigma (sumatoria) y sigma  (integral) en el cálculo de áreas</t>
-  </si>
-  <si>
     <t>Actividad para identificar el significado de los símbolos empleados en la notación respecto a sumatorias e integrales</t>
   </si>
   <si>
@@ -737,9 +728,6 @@
     <t>Refuerza tu aprendizaje: El cálculo de áreas</t>
   </si>
   <si>
-    <t>Actividad para revisar concepciones y aplicaciones del cálculo de áreas</t>
-  </si>
-  <si>
     <t>Plantear una secuencia de preguntas abiertas para que el estudiante concluya cuál es el área de un círculo y de una elipse usando integración</t>
   </si>
   <si>
@@ -831,6 +819,18 @@
   </si>
   <si>
     <t>Los teoremas fundamentales del Cálculo</t>
+  </si>
+  <si>
+    <t>Actividad sobre los métodos de integración</t>
+  </si>
+  <si>
+    <t>Reconoce el significado de sigma (sumatoria) y sigma  (integral) en el cálculo de áreas</t>
+  </si>
+  <si>
+    <t>Actividades sobre el cálculo de áreas</t>
+  </si>
+  <si>
+    <t>Actividad que permite realizar generalizaciones para el cálculo del área entre curvas</t>
   </si>
 </sst>
 </file>
@@ -1122,16 +1122,34 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1171,24 +1189,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1497,9 +1497,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="50.140625" defaultRowHeight="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1507,101 +1507,105 @@
     <col min="1" max="5" width="50.140625" style="20"/>
     <col min="6" max="6" width="50.140625" style="21"/>
     <col min="7" max="7" width="50.140625" style="20"/>
-    <col min="8" max="9" width="50.140625" style="21"/>
-    <col min="10" max="14" width="50.140625" style="20"/>
-    <col min="15" max="17" width="50.140625" style="21"/>
+    <col min="8" max="8" width="11" style="21" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="21" customWidth="1"/>
+    <col min="10" max="10" width="50.140625" style="20"/>
+    <col min="11" max="14" width="0" style="20" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="0" style="21" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="24.5703125" style="21" customWidth="1"/>
+    <col min="17" max="17" width="50.140625" style="21"/>
     <col min="18" max="16384" width="50.140625" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="3" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="42" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="42" t="s">
+      <c r="G1" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="42" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="I1" s="42" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="46" t="s">
+      <c r="J1" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="44" t="s">
+      <c r="K1" s="50" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="42" t="s">
+      <c r="L1" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="48" t="s">
+      <c r="M1" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="48"/>
-      <c r="O1" s="36" t="s">
+      <c r="N1" s="54"/>
+      <c r="O1" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="36" t="s">
+      <c r="P1" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="51" t="s">
+      <c r="Q1" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="55" t="s">
+      <c r="R1" s="40" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="51" t="s">
+      <c r="S1" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="53" t="s">
+      <c r="T1" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="51" t="s">
+      <c r="U1" s="36" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="3" customFormat="1" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="41"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="43"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="49"/>
       <c r="M2" s="22" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="37"/>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="52"/>
-      <c r="R2" s="56"/>
-      <c r="S2" s="52"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="52"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="41"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="37"/>
     </row>
     <row r="3" spans="1:21" s="4" customFormat="1" ht="14.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
@@ -1619,13 +1623,13 @@
       <c r="E3" s="6"/>
       <c r="F3" s="7"/>
       <c r="G3" s="8" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="H3" s="26">
         <v>1</v>
       </c>
       <c r="I3" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J3" s="9" t="s">
         <v>167</v>
@@ -1641,25 +1645,25 @@
       </c>
       <c r="N3" s="30"/>
       <c r="O3" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="P3" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q3" s="15">
         <v>6</v>
       </c>
       <c r="R3" s="16" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="S3" s="15" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="T3" s="17" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="U3" s="15" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:21" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1686,7 +1690,7 @@
         <v>2</v>
       </c>
       <c r="I4" s="27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>156</v>
@@ -1717,7 +1721,7 @@
         <v>141</v>
       </c>
       <c r="T4" s="17" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="U4" s="15" t="s">
         <v>143</v>
@@ -1747,7 +1751,7 @@
         <v>3</v>
       </c>
       <c r="I5" s="27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>160</v>
@@ -1778,7 +1782,7 @@
         <v>141</v>
       </c>
       <c r="T5" s="17" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="U5" s="15" t="s">
         <v>143</v>
@@ -1808,7 +1812,7 @@
         <v>4</v>
       </c>
       <c r="I6" s="27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J6" s="9" t="s">
         <v>162</v>
@@ -1839,7 +1843,7 @@
         <v>141</v>
       </c>
       <c r="T6" s="17" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="U6" s="15" t="s">
         <v>143</v>
@@ -1894,16 +1898,16 @@
         <v>6</v>
       </c>
       <c r="R7" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="S7" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="T7" s="17" t="s">
         <v>219</v>
       </c>
-      <c r="S7" s="15" t="s">
-        <v>220</v>
-      </c>
-      <c r="T7" s="17" t="s">
-        <v>223</v>
-      </c>
       <c r="U7" s="15" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:21" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1930,7 +1934,7 @@
         <v>6</v>
       </c>
       <c r="I8" s="27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J8" s="9" t="s">
         <v>165</v>
@@ -1961,7 +1965,7 @@
         <v>141</v>
       </c>
       <c r="T8" s="17" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="U8" s="15" t="s">
         <v>143</v>
@@ -1991,7 +1995,7 @@
         <v>7</v>
       </c>
       <c r="I9" s="27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J9" s="9" t="s">
         <v>172</v>
@@ -2022,7 +2026,7 @@
         <v>141</v>
       </c>
       <c r="T9" s="17" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="U9" s="15" t="s">
         <v>143</v>
@@ -2052,7 +2056,7 @@
         <v>8</v>
       </c>
       <c r="I10" s="27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J10" s="9" t="s">
         <v>171</v>
@@ -2083,7 +2087,7 @@
         <v>141</v>
       </c>
       <c r="T10" s="17" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="U10" s="15" t="s">
         <v>143</v>
@@ -2113,7 +2117,7 @@
         <v>9</v>
       </c>
       <c r="I11" s="27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J11" s="9" t="s">
         <v>177</v>
@@ -2129,7 +2133,7 @@
         <v>67</v>
       </c>
       <c r="O11" s="7" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="P11" s="14" t="s">
         <v>19</v>
@@ -2144,7 +2148,7 @@
         <v>141</v>
       </c>
       <c r="T11" s="17" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="U11" s="15" t="s">
         <v>143</v>
@@ -2174,10 +2178,10 @@
         <v>10</v>
       </c>
       <c r="I12" s="27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>180</v>
+        <v>245</v>
       </c>
       <c r="K12" s="28" t="s">
         <v>20</v>
@@ -2190,7 +2194,7 @@
         <v>82</v>
       </c>
       <c r="O12" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="P12" s="14" t="s">
         <v>19</v>
@@ -2205,7 +2209,7 @@
         <v>141</v>
       </c>
       <c r="T12" s="17" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="U12" s="15" t="s">
         <v>143</v>
@@ -2229,16 +2233,16 @@
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H13" s="26">
         <v>11</v>
       </c>
       <c r="I13" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="K13" s="28" t="s">
         <v>20</v>
@@ -2247,29 +2251,29 @@
         <v>5</v>
       </c>
       <c r="M13" s="30" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="N13" s="30"/>
       <c r="O13" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="P13" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q13" s="15">
         <v>6</v>
       </c>
       <c r="R13" s="16" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="S13" s="15" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="T13" s="17" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="U13" s="15" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="14" spans="1:21" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2290,16 +2294,16 @@
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="8" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H14" s="26">
         <v>12</v>
       </c>
       <c r="I14" s="27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="K14" s="28" t="s">
         <v>20</v>
@@ -2312,7 +2316,7 @@
         <v>103</v>
       </c>
       <c r="O14" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="P14" s="14" t="s">
         <v>19</v>
@@ -2327,7 +2331,7 @@
         <v>141</v>
       </c>
       <c r="T14" s="17" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="U14" s="15" t="s">
         <v>143</v>
@@ -2351,7 +2355,7 @@
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H15" s="26">
         <v>13</v>
@@ -2376,22 +2380,22 @@
         <v>153</v>
       </c>
       <c r="P15" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q15" s="15">
         <v>6</v>
       </c>
       <c r="R15" s="16" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="S15" s="15" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="T15" s="17" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="U15" s="15" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="16" spans="1:21" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2418,10 +2422,10 @@
         <v>14</v>
       </c>
       <c r="I16" s="27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="K16" s="28" t="s">
         <v>20</v>
@@ -2434,7 +2438,7 @@
         <v>82</v>
       </c>
       <c r="O16" s="7" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="P16" s="14" t="s">
         <v>19</v>
@@ -2449,7 +2453,7 @@
         <v>141</v>
       </c>
       <c r="T16" s="17" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="U16" s="15" t="s">
         <v>143</v>
@@ -2473,7 +2477,7 @@
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="8" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H17" s="26">
         <v>15</v>
@@ -2482,7 +2486,7 @@
         <v>20</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="K17" s="28" t="s">
         <v>20</v>
@@ -2495,10 +2499,10 @@
         <v>96</v>
       </c>
       <c r="O17" s="7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="P17" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q17" s="15">
         <v>6</v>
@@ -2510,7 +2514,7 @@
         <v>141</v>
       </c>
       <c r="T17" s="17" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="U17" s="15" t="s">
         <v>143</v>
@@ -2534,16 +2538,16 @@
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="8" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H18" s="26">
         <v>16</v>
       </c>
       <c r="I18" s="27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="K18" s="28" t="s">
         <v>20</v>
@@ -2556,7 +2560,7 @@
         <v>67</v>
       </c>
       <c r="O18" s="7" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="P18" s="14" t="s">
         <v>19</v>
@@ -2571,7 +2575,7 @@
         <v>141</v>
       </c>
       <c r="T18" s="17" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="U18" s="15" t="s">
         <v>143</v>
@@ -2595,16 +2599,16 @@
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="8" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H19" s="26">
         <v>17</v>
       </c>
       <c r="I19" s="27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="K19" s="28" t="s">
         <v>20</v>
@@ -2617,7 +2621,7 @@
         <v>82</v>
       </c>
       <c r="O19" s="7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="P19" s="14" t="s">
         <v>19</v>
@@ -2632,7 +2636,7 @@
         <v>141</v>
       </c>
       <c r="T19" s="17" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="U19" s="15" t="s">
         <v>143</v>
@@ -2649,12 +2653,12 @@
         <v>123</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="7"/>
       <c r="G20" s="8" t="s">
-        <v>210</v>
+        <v>246</v>
       </c>
       <c r="H20" s="26">
         <v>18</v>
@@ -2663,7 +2667,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="K20" s="28" t="s">
         <v>20</v>
@@ -2676,10 +2680,10 @@
         <v>69</v>
       </c>
       <c r="O20" s="7" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="P20" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q20" s="15">
         <v>6</v>
@@ -2691,7 +2695,7 @@
         <v>141</v>
       </c>
       <c r="T20" s="17" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="U20" s="15" t="s">
         <v>143</v>
@@ -2708,12 +2712,12 @@
         <v>123</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="7"/>
       <c r="G21" s="8" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="H21" s="26">
         <v>19</v>
@@ -2722,7 +2726,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="9" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="K21" s="28" t="s">
         <v>20</v>
@@ -2735,10 +2739,10 @@
         <v>84</v>
       </c>
       <c r="O21" s="7" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="P21" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q21" s="15">
         <v>6</v>
@@ -2750,7 +2754,7 @@
         <v>141</v>
       </c>
       <c r="T21" s="17" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="U21" s="15" t="s">
         <v>143</v>
@@ -2767,23 +2771,23 @@
         <v>123</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>128</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="8" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="H22" s="26">
         <v>20</v>
       </c>
       <c r="I22" s="27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>217</v>
+        <v>247</v>
       </c>
       <c r="K22" s="28" t="s">
         <v>20</v>
@@ -2796,7 +2800,7 @@
         <v>82</v>
       </c>
       <c r="O22" s="7" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="P22" s="14" t="s">
         <v>19</v>
@@ -2811,7 +2815,7 @@
         <v>141</v>
       </c>
       <c r="T22" s="17" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="U22" s="15" t="s">
         <v>143</v>
@@ -2828,23 +2832,23 @@
         <v>123</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>128</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H23" s="26">
         <v>21</v>
       </c>
       <c r="I23" s="27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J23" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K23" s="28" t="s">
         <v>20</v>
@@ -2855,7 +2859,7 @@
       </c>
       <c r="N23" s="30"/>
       <c r="O23" s="7" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="P23" s="14" t="s">
         <v>20</v>
@@ -2864,16 +2868,16 @@
         <v>6</v>
       </c>
       <c r="R23" s="16" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="S23" s="15" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="T23" s="17" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="U23" s="15" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="24" spans="1:21" s="4" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2892,16 +2896,16 @@
       <c r="E24" s="11"/>
       <c r="F24" s="12"/>
       <c r="G24" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H24" s="26">
         <v>22</v>
       </c>
       <c r="I24" s="27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>195</v>
+        <v>248</v>
       </c>
       <c r="K24" s="28" t="s">
         <v>20</v>
@@ -2914,7 +2918,7 @@
         <v>84</v>
       </c>
       <c r="O24" s="19" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="P24" s="14" t="s">
         <v>19</v>
@@ -2959,10 +2963,10 @@
         <v>23</v>
       </c>
       <c r="I25" s="27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J25" s="18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K25" s="28" t="s">
         <v>20</v>
@@ -3006,10 +3010,10 @@
         <v>24</v>
       </c>
       <c r="I26" s="27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J26" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K26" s="28" t="s">
         <v>20</v>
@@ -3022,7 +3026,7 @@
         <v>103</v>
       </c>
       <c r="O26" s="19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="P26" s="14" t="s">
         <v>19</v>
@@ -3037,7 +3041,7 @@
         <v>141</v>
       </c>
       <c r="T26" s="17" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="U26" s="15" t="s">
         <v>143</v>
@@ -3061,7 +3065,7 @@
       </c>
       <c r="F27" s="12"/>
       <c r="G27" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H27" s="26">
         <v>25</v>
@@ -3070,7 +3074,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="18" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K27" s="28" t="s">
         <v>20</v>
@@ -3083,7 +3087,7 @@
         <v>83</v>
       </c>
       <c r="O27" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="P27" s="14" t="s">
         <v>20</v>
@@ -3098,7 +3102,7 @@
         <v>141</v>
       </c>
       <c r="T27" s="17" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="U27" s="15" t="s">
         <v>143</v>
@@ -3294,12 +3298,6 @@
     <filterColumn colId="12" showButton="0"/>
   </autoFilter>
   <mergeCells count="20">
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -3314,6 +3312,12 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3336,7 +3340,7 @@
           <x14:formula1>
             <xm:f>DATOS!$D$1:$D$2</xm:f>
           </x14:formula1>
-          <xm:sqref>K3:K27 P3:P27 I3:I27</xm:sqref>
+          <xm:sqref>K3:K27 I3:I27 P3:P27</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>